<commit_message>
make tomb id uniform across imgs and table
</commit_message>
<xml_diff>
--- a/src/assets/cemetery_table.xlsx
+++ b/src/assets/cemetery_table.xlsx
@@ -453,7 +453,7 @@
     <t xml:space="preserve">Ne en 1886</t>
   </si>
   <si>
-    <t>A01</t>
+    <t>A1</t>
   </si>
   <si>
     <t>Renée</t>
@@ -1053,7 +1053,7 @@
     <t>01.11.1934</t>
   </si>
   <si>
-    <t>C06</t>
+    <t>C6</t>
   </si>
   <si>
     <t>19.3.1950</t>
@@ -1194,7 +1194,7 @@
     <t>Tamam</t>
   </si>
   <si>
-    <t>B05</t>
+    <t>B5</t>
   </si>
   <si>
     <t xml:space="preserve"> Née a Tyr</t>
@@ -1215,7 +1215,7 @@
     <t>25.2.1955</t>
   </si>
   <si>
-    <t>A06</t>
+    <t>A6</t>
   </si>
   <si>
     <t>Malakeh</t>
@@ -2532,7 +2532,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A86" zoomScale="100" workbookViewId="0">
       <selection activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix death date Balaciano
</commit_message>
<xml_diff>
--- a/src/assets/cemetery_table.xlsx
+++ b/src/assets/cemetery_table.xlsx
@@ -99,7 +99,7 @@
     <t>BALACIANO</t>
   </si>
   <si>
-    <t>26.1.3776</t>
+    <t>26.1.1876</t>
   </si>
   <si>
     <t>D41</t>
@@ -2532,7 +2532,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A86" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>